<commit_message>
workaround for Bug in FastFormularProcessor. LongArgumentListSupportingStandardFormularProcessor now supports "+"-concatenation in nested loops
</commit_message>
<xml_diff>
--- a/src/test/resources/jxls-test.xlsx
+++ b/src/test/resources/jxls-test.xlsx
@@ -36,9 +36,33 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Segoe UI"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
-          <t>jx:area(lastCell="B8")</t>
+          <t>jx:area(lastCell="B11")</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hombergs, Tom:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="departments" var="department" lastCell="B8")</t>
         </r>
       </text>
     </comment>
@@ -51,7 +75,7 @@
             <rFont val="Segoe UI"/>
             <family val="2"/>
           </rPr>
-          <t>jx:each(items="employees" var="employee" lastCell="B5")</t>
+          <t>jx:each(items="department.employees" var="employee" lastCell="B5")</t>
         </r>
       </text>
     </comment>
@@ -60,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -87,6 +111,24 @@
   </si>
   <si>
     <t>${employee.bonus}</t>
+  </si>
+  <si>
+    <t>Department Sum Salary:</t>
+  </si>
+  <si>
+    <t>Department Sum Bonus:</t>
+  </si>
+  <si>
+    <t>Department:</t>
+  </si>
+  <si>
+    <t>${department.name}</t>
+  </si>
+  <si>
+    <t>$[SUM(B6)]</t>
+  </si>
+  <si>
+    <t>$[SUM(B7)]</t>
   </si>
 </sst>
 </file>
@@ -113,9 +155,10 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Segoe UI"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Segoe UI"/>
@@ -142,9 +185,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -456,19 +502,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>0</v>
@@ -478,7 +532,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
@@ -486,25 +540,44 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>7</v>
+      <c r="B11" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>